<commit_message>
added readme information and minor bug fix
</commit_message>
<xml_diff>
--- a/data/simulations/raw/test_01.xlsx
+++ b/data/simulations/raw/test_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erlbo\PycharmProjects\catapult-experiment-uncertained\data\simulations\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1919E621-841D-4AC6-B4DB-2E1541BB3BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC85BEBC-E9B4-450E-BC59-1D96B28F0DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7E3CF10E-263F-40D5-BCB5-46A3505E6E5C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{7E3CF10E-263F-40D5-BCB5-46A3505E6E5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,12 +154,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -175,12 +181,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11322,7 +11329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED0F4C4-FCA4-49D1-B66A-59D885B6D1E4}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -11401,13 +11408,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4489FB5F-CFC6-48AE-BCB7-44C6553E03A8}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="14" width="9.88671875" customWidth="1"/>
+    <col min="1" max="13" width="9.88671875" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -11450,7 +11458,7 @@
       <c r="M1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -11494,7 +11502,7 @@
       <c r="M2">
         <v>0.05</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="3">
         <f>0.05*30</f>
         <v>1.5</v>
       </c>

</xml_diff>